<commit_message>
🔁 Add election-data.json and finalize MongoDB integration
</commit_message>
<xml_diff>
--- a/data.csv.xlsx
+++ b/data.csv.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4d4647ffad6c4b65/Desktop/Aaryan/nic design/election-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{223516C3-5904-4073-9D3A-9FC0D415AE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{223516C3-5904-4073-9D3A-9FC0D415AE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DBE7774-3168-46C2-85FA-43B2C3CD2965}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{60109702-0A2B-453B-B2F0-CED9105C2020}"/>
   </bookViews>
@@ -664,6 +664,7 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -835,7 +836,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -919,7 +920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -935,7 +936,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -955,7 +956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
@@ -975,7 +976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
@@ -1015,7 +1016,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
@@ -1031,7 +1032,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
@@ -1051,7 +1052,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>43</v>
       </c>
@@ -1087,7 +1088,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>45</v>
       </c>
@@ -1159,7 +1160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>49</v>
       </c>
@@ -1195,7 +1196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
         <v>52</v>
       </c>
@@ -1227,7 +1228,7 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
         <v>54</v>
       </c>
@@ -1263,7 +1264,7 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
         <v>56</v>
       </c>
@@ -1283,7 +1284,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
         <v>57</v>
       </c>
@@ -1299,7 +1300,7 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
         <v>58</v>
       </c>

</xml_diff>